<commit_message>
Prep for mtg with AMN, AC
</commit_message>
<xml_diff>
--- a/analysis/data/xlsx/Raw_Sorting_Data_151102.xlsx
+++ b/analysis/data/xlsx/Raw_Sorting_Data_151102.xlsx
@@ -538,8 +538,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -555,9 +557,11 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -31488,7 +31492,7 @@
   <dimension ref="A1:W164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
@@ -43326,11 +43330,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W161"/>
+  <dimension ref="A1:W159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162:XFD689"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C164" sqref="C164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -48158,7 +48162,7 @@
         <v>0</v>
       </c>
       <c r="W67">
-        <f t="shared" ref="W67:W135" si="1">SUMIF(C67:V67,"&lt;&gt;",C67:V67)</f>
+        <f t="shared" ref="W67:W128" si="1">SUMIF(C67:V67,"&lt;&gt;",C67:V67)</f>
         <v>4</v>
       </c>
     </row>
@@ -52622,7 +52626,7 @@
         <v>1</v>
       </c>
       <c r="W129">
-        <f t="shared" si="1"/>
+        <f>SUM(C129:V129)</f>
         <v>2</v>
       </c>
     </row>
@@ -52694,7 +52698,7 @@
         <v>0</v>
       </c>
       <c r="W130">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="W130:W134" si="2">SUM(C130:V130)</f>
         <v>1</v>
       </c>
     </row>
@@ -52766,7 +52770,7 @@
         <v>0</v>
       </c>
       <c r="W131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -52838,7 +52842,7 @@
         <v>0</v>
       </c>
       <c r="W132">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -52910,7 +52914,7 @@
         <v>1</v>
       </c>
       <c r="W133">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -52982,31 +52986,31 @@
         <v>0</v>
       </c>
       <c r="W134">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:23">
       <c r="A135">
-        <v>8017</v>
+        <v>8018</v>
       </c>
       <c r="B135">
         <v>134</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135">
         <v>0</v>
       </c>
       <c r="G135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H135">
         <v>0</v>
@@ -53018,7 +53022,7 @@
         <v>0</v>
       </c>
       <c r="K135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L135">
         <v>0</v>
@@ -53030,7 +53034,7 @@
         <v>0</v>
       </c>
       <c r="O135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P135">
         <v>0</v>
@@ -53048,14 +53052,14 @@
         <v>0</v>
       </c>
       <c r="U135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V135">
         <v>0</v>
       </c>
       <c r="W135">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="W135:W159" si="3">SUMIF(C135:V135,"&lt;&gt;",C135:V135)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:23">
@@ -53066,19 +53070,19 @@
         <v>135</v>
       </c>
       <c r="C136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D136">
         <v>0</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F136">
         <v>0</v>
       </c>
       <c r="G136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -53090,7 +53094,7 @@
         <v>0</v>
       </c>
       <c r="K136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L136">
         <v>0</v>
@@ -53102,32 +53106,32 @@
         <v>0</v>
       </c>
       <c r="O136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q136">
         <v>0</v>
       </c>
       <c r="R136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S136">
         <v>0</v>
       </c>
       <c r="T136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U136">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W136">
-        <f t="shared" ref="W136:W161" si="2">SUMIF(C136:V136,"&lt;&gt;",C136:V136)</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="137" spans="1:23">
@@ -53156,7 +53160,7 @@
         <v>0</v>
       </c>
       <c r="I137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J137">
         <v>0</v>
@@ -53177,29 +53181,29 @@
         <v>0</v>
       </c>
       <c r="P137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S137">
         <v>0</v>
       </c>
       <c r="T137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U137">
         <v>0</v>
       </c>
       <c r="V137">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W137">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:23">
@@ -53213,7 +53217,7 @@
         <v>0</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138">
         <v>0</v>
@@ -53222,16 +53226,16 @@
         <v>0</v>
       </c>
       <c r="G138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H138">
         <v>0</v>
       </c>
       <c r="I138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K138">
         <v>0</v>
@@ -53252,7 +53256,7 @@
         <v>0</v>
       </c>
       <c r="Q138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R138">
         <v>0</v>
@@ -53270,8 +53274,8 @@
         <v>0</v>
       </c>
       <c r="W138">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:23">
@@ -53285,16 +53289,16 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E139">
         <v>0</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H139">
         <v>0</v>
@@ -53303,7 +53307,7 @@
         <v>0</v>
       </c>
       <c r="J139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K139">
         <v>0</v>
@@ -53312,7 +53316,7 @@
         <v>0</v>
       </c>
       <c r="M139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N139">
         <v>0</v>
@@ -53330,7 +53334,7 @@
         <v>0</v>
       </c>
       <c r="S139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T139">
         <v>0</v>
@@ -53342,7 +53346,7 @@
         <v>0</v>
       </c>
       <c r="W139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -53363,7 +53367,7 @@
         <v>0</v>
       </c>
       <c r="F140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G140">
         <v>0</v>
@@ -53381,13 +53385,13 @@
         <v>0</v>
       </c>
       <c r="L140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O140">
         <v>0</v>
@@ -53402,7 +53406,7 @@
         <v>0</v>
       </c>
       <c r="S140">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T140">
         <v>0</v>
@@ -53414,13 +53418,13 @@
         <v>0</v>
       </c>
       <c r="W140">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:23">
       <c r="A141">
-        <v>8018</v>
+        <v>8019</v>
       </c>
       <c r="B141">
         <v>140</v>
@@ -53447,7 +53451,7 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K141">
         <v>0</v>
@@ -53459,7 +53463,7 @@
         <v>0</v>
       </c>
       <c r="N141">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O141">
         <v>0</v>
@@ -53480,14 +53484,14 @@
         <v>0</v>
       </c>
       <c r="U141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W141">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f>SUM(C141:V141)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="142" spans="1:23">
@@ -53498,7 +53502,7 @@
         <v>141</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -53519,16 +53523,16 @@
         <v>0</v>
       </c>
       <c r="J142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N142">
         <v>0</v>
@@ -53552,14 +53556,14 @@
         <v>0</v>
       </c>
       <c r="U142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V142">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W142">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" ref="W142:W146" si="4">SUM(C142:V142)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:23">
@@ -53570,7 +53574,7 @@
         <v>142</v>
       </c>
       <c r="C143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -53594,13 +53598,13 @@
         <v>0</v>
       </c>
       <c r="K143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L143">
         <v>0</v>
       </c>
       <c r="M143">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N143">
         <v>0</v>
@@ -53612,7 +53616,7 @@
         <v>0</v>
       </c>
       <c r="Q143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R143">
         <v>0</v>
@@ -53621,7 +53625,7 @@
         <v>0</v>
       </c>
       <c r="T143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U143">
         <v>0</v>
@@ -53630,8 +53634,8 @@
         <v>0</v>
       </c>
       <c r="W143">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:23">
@@ -53645,7 +53649,7 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144">
         <v>0</v>
@@ -53654,13 +53658,13 @@
         <v>0</v>
       </c>
       <c r="G144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H144">
         <v>0</v>
       </c>
       <c r="I144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J144">
         <v>0</v>
@@ -53684,7 +53688,7 @@
         <v>0</v>
       </c>
       <c r="Q144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R144">
         <v>0</v>
@@ -53693,7 +53697,7 @@
         <v>0</v>
       </c>
       <c r="T144">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U144">
         <v>0</v>
@@ -53702,8 +53706,8 @@
         <v>0</v>
       </c>
       <c r="W144">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:23">
@@ -53711,13 +53715,13 @@
         <v>8019</v>
       </c>
       <c r="B145">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C145">
         <v>0</v>
       </c>
       <c r="D145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E145">
         <v>0</v>
@@ -53726,13 +53730,13 @@
         <v>0</v>
       </c>
       <c r="G145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I145">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J145">
         <v>0</v>
@@ -53750,19 +53754,19 @@
         <v>0</v>
       </c>
       <c r="O145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q145">
         <v>0</v>
       </c>
       <c r="R145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T145">
         <v>0</v>
@@ -53774,8 +53778,8 @@
         <v>0</v>
       </c>
       <c r="W145">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:23">
@@ -53783,7 +53787,7 @@
         <v>8019</v>
       </c>
       <c r="B146">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -53801,7 +53805,7 @@
         <v>0</v>
       </c>
       <c r="H146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I146">
         <v>0</v>
@@ -53819,22 +53823,22 @@
         <v>0</v>
       </c>
       <c r="N146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q146">
         <v>0</v>
       </c>
       <c r="R146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S146">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T146">
         <v>0</v>
@@ -53846,8 +53850,8 @@
         <v>0</v>
       </c>
       <c r="W146">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:23">
@@ -53864,10 +53868,10 @@
         <v>0</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G147">
         <v>0</v>
@@ -53891,7 +53895,7 @@
         <v>0</v>
       </c>
       <c r="N147">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O147">
         <v>0</v>
@@ -53918,28 +53922,28 @@
         <v>0</v>
       </c>
       <c r="W147">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:23">
       <c r="A148">
-        <v>8019</v>
+        <v>8020</v>
       </c>
       <c r="B148">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C148">
         <v>0</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F148">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G148">
         <v>0</v>
@@ -53975,7 +53979,7 @@
         <v>0</v>
       </c>
       <c r="R148">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S148">
         <v>0</v>
@@ -53990,7 +53994,7 @@
         <v>0</v>
       </c>
       <c r="W148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -53999,10 +54003,10 @@
         <v>8020</v>
       </c>
       <c r="B149">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D149">
         <v>0</v>
@@ -54014,10 +54018,10 @@
         <v>0</v>
       </c>
       <c r="G149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I149">
         <v>0</v>
@@ -54053,7 +54057,7 @@
         <v>0</v>
       </c>
       <c r="T149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U149">
         <v>0</v>
@@ -54062,8 +54066,8 @@
         <v>0</v>
       </c>
       <c r="W149">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
     </row>
     <row r="150" spans="1:23">
@@ -54071,13 +54075,13 @@
         <v>8020</v>
       </c>
       <c r="B150">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C150">
         <v>0</v>
       </c>
       <c r="D150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E150">
         <v>0</v>
@@ -54101,7 +54105,7 @@
         <v>0</v>
       </c>
       <c r="L150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M150">
         <v>0</v>
@@ -54110,7 +54114,7 @@
         <v>0</v>
       </c>
       <c r="O150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P150">
         <v>0</v>
@@ -54119,7 +54123,7 @@
         <v>0</v>
       </c>
       <c r="R150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S150">
         <v>0</v>
@@ -54134,7 +54138,7 @@
         <v>0</v>
       </c>
       <c r="W150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -54143,10 +54147,10 @@
         <v>8020</v>
       </c>
       <c r="B151">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -54158,16 +54162,16 @@
         <v>0</v>
       </c>
       <c r="G151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I151">
         <v>0</v>
       </c>
       <c r="J151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K151">
         <v>0</v>
@@ -54197,17 +54201,17 @@
         <v>0</v>
       </c>
       <c r="T151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U151">
         <v>0</v>
       </c>
       <c r="V151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W151">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:23">
@@ -54215,7 +54219,7 @@
         <v>8020</v>
       </c>
       <c r="B152">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -54224,7 +54228,7 @@
         <v>0</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F152">
         <v>0</v>
@@ -54245,7 +54249,7 @@
         <v>0</v>
       </c>
       <c r="L152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M152">
         <v>0</v>
@@ -54254,13 +54258,13 @@
         <v>0</v>
       </c>
       <c r="O152">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P152">
         <v>0</v>
       </c>
       <c r="Q152">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R152">
         <v>0</v>
@@ -54278,7 +54282,7 @@
         <v>0</v>
       </c>
       <c r="W152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -54287,7 +54291,7 @@
         <v>8020</v>
       </c>
       <c r="B153">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C153">
         <v>0</v>
@@ -54311,7 +54315,7 @@
         <v>0</v>
       </c>
       <c r="J153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K153">
         <v>0</v>
@@ -54329,7 +54333,7 @@
         <v>0</v>
       </c>
       <c r="P153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q153">
         <v>0</v>
@@ -54344,13 +54348,13 @@
         <v>0</v>
       </c>
       <c r="U153">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V153">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -54359,7 +54363,7 @@
         <v>8020</v>
       </c>
       <c r="B154">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -54368,7 +54372,7 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F154">
         <v>0</v>
@@ -54380,7 +54384,7 @@
         <v>0</v>
       </c>
       <c r="I154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J154">
         <v>0</v>
@@ -54404,13 +54408,13 @@
         <v>0</v>
       </c>
       <c r="Q154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R154">
         <v>0</v>
       </c>
       <c r="S154">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T154">
         <v>0</v>
@@ -54422,7 +54426,7 @@
         <v>0</v>
       </c>
       <c r="W154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -54431,7 +54435,7 @@
         <v>8020</v>
       </c>
       <c r="B155">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -54467,13 +54471,13 @@
         <v>0</v>
       </c>
       <c r="N155">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O155">
         <v>0</v>
       </c>
       <c r="P155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q155">
         <v>0</v>
@@ -54488,14 +54492,14 @@
         <v>0</v>
       </c>
       <c r="U155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V155">
         <v>0</v>
       </c>
       <c r="W155">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:23">
@@ -54503,7 +54507,7 @@
         <v>8020</v>
       </c>
       <c r="B156">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -54515,7 +54519,7 @@
         <v>0</v>
       </c>
       <c r="F156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G156">
         <v>0</v>
@@ -54524,19 +54528,19 @@
         <v>0</v>
       </c>
       <c r="I156">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J156">
         <v>0</v>
       </c>
       <c r="K156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L156">
         <v>0</v>
       </c>
       <c r="M156">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N156">
         <v>0</v>
@@ -54554,7 +54558,7 @@
         <v>0</v>
       </c>
       <c r="S156">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T156">
         <v>0</v>
@@ -54566,31 +54570,31 @@
         <v>0</v>
       </c>
       <c r="W156">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:23">
       <c r="A157">
-        <v>8020</v>
+        <v>8021</v>
       </c>
       <c r="B157">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C157">
         <v>0</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -54602,7 +54606,7 @@
         <v>0</v>
       </c>
       <c r="K157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L157">
         <v>0</v>
@@ -54611,7 +54615,7 @@
         <v>0</v>
       </c>
       <c r="N157">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O157">
         <v>0</v>
@@ -54620,7 +54624,7 @@
         <v>0</v>
       </c>
       <c r="Q157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R157">
         <v>0</v>
@@ -54629,25 +54633,25 @@
         <v>0</v>
       </c>
       <c r="T157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V157">
         <v>0</v>
       </c>
       <c r="W157">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:23">
       <c r="A158">
-        <v>8020</v>
+        <v>8021</v>
       </c>
       <c r="B158">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -54659,46 +54663,46 @@
         <v>0</v>
       </c>
       <c r="F158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G158">
         <v>0</v>
       </c>
       <c r="H158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J158">
         <v>0</v>
       </c>
       <c r="K158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L158">
         <v>0</v>
       </c>
       <c r="M158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O158">
         <v>0</v>
       </c>
       <c r="P158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q158">
         <v>0</v>
       </c>
       <c r="R158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S158">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T158">
         <v>0</v>
@@ -54710,8 +54714,8 @@
         <v>0</v>
       </c>
       <c r="W158">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
     </row>
     <row r="159" spans="1:23">
@@ -54719,22 +54723,22 @@
         <v>8021</v>
       </c>
       <c r="B159">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H159">
         <v>0</v>
@@ -54743,28 +54747,28 @@
         <v>0</v>
       </c>
       <c r="J159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N159">
         <v>0</v>
       </c>
       <c r="O159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P159">
         <v>0</v>
       </c>
       <c r="Q159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R159">
         <v>0</v>
@@ -54773,160 +54777,16 @@
         <v>0</v>
       </c>
       <c r="T159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W159">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:23">
-      <c r="A160">
-        <v>8021</v>
-      </c>
-      <c r="B160">
-        <v>160</v>
-      </c>
-      <c r="C160">
-        <v>0</v>
-      </c>
-      <c r="D160">
-        <v>0</v>
-      </c>
-      <c r="E160">
-        <v>0</v>
-      </c>
-      <c r="F160">
-        <v>0</v>
-      </c>
-      <c r="G160">
-        <v>0</v>
-      </c>
-      <c r="H160">
-        <v>1</v>
-      </c>
-      <c r="I160">
-        <v>1</v>
-      </c>
-      <c r="J160">
-        <v>0</v>
-      </c>
-      <c r="K160">
-        <v>0</v>
-      </c>
-      <c r="L160">
-        <v>0</v>
-      </c>
-      <c r="M160">
-        <v>0</v>
-      </c>
-      <c r="N160">
-        <v>1</v>
-      </c>
-      <c r="O160">
-        <v>0</v>
-      </c>
-      <c r="P160">
-        <v>1</v>
-      </c>
-      <c r="Q160">
-        <v>0</v>
-      </c>
-      <c r="R160">
-        <v>1</v>
-      </c>
-      <c r="S160">
-        <v>1</v>
-      </c>
-      <c r="T160">
-        <v>0</v>
-      </c>
-      <c r="U160">
-        <v>0</v>
-      </c>
-      <c r="V160">
-        <v>0</v>
-      </c>
-      <c r="W160">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="161" spans="1:23">
-      <c r="A161">
-        <v>8021</v>
-      </c>
-      <c r="B161">
-        <v>161</v>
-      </c>
-      <c r="C161">
-        <v>1</v>
-      </c>
-      <c r="D161">
-        <v>0</v>
-      </c>
-      <c r="E161">
-        <v>0</v>
-      </c>
-      <c r="F161">
-        <v>0</v>
-      </c>
-      <c r="G161">
-        <v>0</v>
-      </c>
-      <c r="H161">
-        <v>0</v>
-      </c>
-      <c r="I161">
-        <v>0</v>
-      </c>
-      <c r="J161">
-        <v>1</v>
-      </c>
-      <c r="K161">
-        <v>0</v>
-      </c>
-      <c r="L161">
-        <v>1</v>
-      </c>
-      <c r="M161">
-        <v>1</v>
-      </c>
-      <c r="N161">
-        <v>0</v>
-      </c>
-      <c r="O161">
-        <v>1</v>
-      </c>
-      <c r="P161">
-        <v>0</v>
-      </c>
-      <c r="Q161">
-        <v>0</v>
-      </c>
-      <c r="R161">
-        <v>0</v>
-      </c>
-      <c r="S161">
-        <v>0</v>
-      </c>
-      <c r="T161">
-        <v>0</v>
-      </c>
-      <c r="U161">
-        <v>0</v>
-      </c>
-      <c r="V161">
-        <v>1</v>
-      </c>
-      <c r="W161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
@@ -54941,6 +54801,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="C1:V1" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>